<commit_message>
Updated Sprint Protocol 1
</commit_message>
<xml_diff>
--- a/protocols/sprint_protocol_1.xlsx
+++ b/protocols/sprint_protocol_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f4cd42c82715d1a/Dokumente/bif/itp/studyhelp/protocols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\studyhelp\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D64EEBBD-AA4F-4C7A-8D1F-28D034097BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567CE5AE-5CE9-4217-AA46-8BC37325889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="500" windowWidth="14400" windowHeight="7810" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -129,7 +129,16 @@
     <t>Creating basic CSS stylesheet</t>
   </si>
   <si>
-    <t>29.03.2022, 12:00</t>
+    <t>Wir haben erstmals ein paar Templates für die index.html Seite erstellt, die später noch verändert werden können (WiP)</t>
+  </si>
+  <si>
+    <t>Das Ändern von Bootstrap Eigenschaften ist mit dem Bearbeiten vom Source Code verbunden, aus diesem Grund belassen wir vorerst es bei Vanilla Bootstrap (WiP)</t>
+  </si>
+  <si>
+    <t>Zusammen mit der organisatorischen Herausforderung, Git und Github einzurichten, hat das Erstellen der Projektstruktur relativ viel Zeit in Anspruch genommen (Done)</t>
+  </si>
+  <si>
+    <t>29.03.2022, 19:30</t>
   </si>
 </sst>
 </file>
@@ -381,17 +390,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -399,47 +414,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -769,33 +778,33 @@
     <col min="4" max="4" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.453125" style="2"/>
-    <col min="8" max="8" width="34.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="153.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="5"/>
@@ -809,10 +818,10 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="18">
         <v>1</v>
       </c>
@@ -822,12 +831,12 @@
       <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -835,10 +844,10 @@
       <c r="G5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="20">
         <v>21</v>
       </c>
@@ -848,10 +857,10 @@
       <c r="G6" s="21"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="22" t="s">
         <v>23</v>
       </c>
@@ -861,81 +870,81 @@
       <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -974,15 +983,17 @@
         <v>5</v>
       </c>
       <c r="D16" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="9">
         <f>D16-C16</f>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
@@ -994,14 +1005,18 @@
       <c r="C17" s="7">
         <v>15</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7">
+        <v>4</v>
+      </c>
       <c r="E17" s="9">
         <f t="shared" ref="E17:E25" si="0">D17-C17</f>
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
@@ -1013,14 +1028,18 @@
       <c r="C18" s="7">
         <v>15</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
       <c r="E18" s="9">
         <f t="shared" si="0"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
@@ -1137,7 +1156,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
-        <v>-33</v>
+        <v>-25</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -1162,6 +1181,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
@@ -1178,10 +1201,6 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>